<commit_message>
break fix from MBHS-1289
</commit_message>
<xml_diff>
--- a/caseTypeMapping.xlsx
+++ b/caseTypeMapping.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3127CAE2-D718-431D-A802-EC4F01830D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{3127CAE2-D718-431D-A802-EC4F01830D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4767A39B-5C25-4EDD-AF06-02A3A7139DA7}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1815" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Code</t>
   </si>
@@ -46,15 +46,9 @@
     <t>Mapping</t>
   </si>
   <si>
-    <t>case type desc</t>
-  </si>
-  <si>
     <t>UNMAPPED</t>
   </si>
   <si>
-    <t>sssss</t>
-  </si>
-  <si>
     <t>EXCLUDE</t>
   </si>
   <si>
@@ -143,6 +137,9 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>playwright, aqa test for upload mapping</t>
   </si>
 </sst>
 </file>
@@ -522,17 +519,17 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="3" width="100" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -546,26 +543,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1111111</v>
+        <v>76543</v>
       </c>
       <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>123</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -580,161 +571,161 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>